<commit_message>
phew almost screwed it all up
</commit_message>
<xml_diff>
--- a/pdfs/account_info.xlsx
+++ b/pdfs/account_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,28 +521,6 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Eric</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>5000</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Bank Account</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>